<commit_message>
Updates per sprint 5 discussions
</commit_message>
<xml_diff>
--- a/docs/14c Phase 2 Implementation Plan - Milestone Sprint View.xlsx
+++ b/docs/14c Phase 2 Implementation Plan - Milestone Sprint View.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="423" documentId="E50BC0C45E0ECAE6C6A77992721E318C7FF34092" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{02B56172-BD1D-4C73-BEA6-85F7DBEE1619}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="11340" windowHeight="4755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="11340" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Striegel, Elizabeth R - WHD</author>
   </authors>
   <commentList>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{CC8E7621-FD0E-496E-9FB5-81D2F17AD214}">
+    <comment ref="D7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -251,6 +250,47 @@
 11/8-11/21</t>
   </si>
   <si>
+    <t>Internal application screen review (Policy/WHD front office/SOL)
+Help desk details
+Verify signature needs on first page. Are there issues if the preparer filles out the signature? (add to github)</t>
+  </si>
+  <si>
+    <t>Sprint 5
+11/22-12/5</t>
+  </si>
+  <si>
+    <t>PRA submission to OMB</t>
+  </si>
+  <si>
+    <t>DECEMBER</t>
+  </si>
+  <si>
+    <t>Stabilize, Knowledge Transfer, Final Demo/Deploy in DOL</t>
+  </si>
+  <si>
+    <t>QA Testing</t>
+  </si>
+  <si>
+    <t>Sprint 6
+12/6-12/19</t>
+  </si>
+  <si>
+    <t>Demo/Validation of acceptance criteria.</t>
+  </si>
+  <si>
+    <t>Sprint 7
+12/20-1/2</t>
+  </si>
+  <si>
+    <t>critical/ATO Defect fixes done. App deployed in DOL Dev.</t>
+  </si>
+  <si>
+    <t>END OF POP</t>
+  </si>
+  <si>
+    <t>All requirements and acceptance criteria met. App deployed in DOL dev. Knowledge transfer complete. All critical/major defects (ATO, features) are addressed.</t>
+  </si>
+  <si>
     <t xml:space="preserve">
 PDF Attachment
 email Api: Write story (needs to be written, dependency to #166)
@@ -273,40 +313,42 @@
 Uploaded files are secured: https://github.com/18F/dol-whd-14c/issues/174
 User session inactivity: https://github.com/18F/dol-whd-14c/issues/76
 WHD needs to provide requirements
-</t>
+• Login workflow (#341). Bug blocking accessibility stories</t>
+  </si>
+  <si>
+    <t>Notes for grooming 11/15:
+• #390: Is this just a placeholder? All implementation stories for login workflow are in Ready to Start.
+• #388 and #166: Are these now dups as well and can they be cleaned up?
+• Verify that uploading files and virus scanning is complete
+• User testing behind in week Sprint 4 due to outreach</t>
   </si>
   <si>
     <t>Accessibility remediation:
 https://github.com/18F/dol-whd-14c/issues/296 (in progress from previous sprint)
-https://github.com/18F/dol-whd-14c/issues/299
-https://github.com/18F/dol-whd-14c/issues/297
+https://github.com/18F/dol-whd-14c/issues/299 (moved to next sprint)
+https://github.com/18F/dol-whd-14c/issues/297 (continued in next sprint)
 Research:
 • Registration, continued(#380)
 • Signature on first page (need to hear from policy first)
 • QA Testing epics (stakeholder/end users/etc):
 • Wage Data (#394) #340 epic
+Visual Design + Implementation:
 Changing my password
 • https://github.com/18F/dol-whd-14c/issues/69
-Visual Design + Implementation:
 • Global helpdesk visuals (#381)
+• Session timeout (#76)
 • Instruction language added
 https://github.com/18F/dol-whd-14c/issues/304
 https://github.com/18F/dol-whd-14c/issues/303
 • Banner (#81)
-• Session timeout (#76)
 • Login workflow (#341)</t>
   </si>
   <si>
-    <t>Internal application screen review (Policy/WHD front office/SOL)
-Help desk details
-Verify signature needs on first page. Are there issues if the preparer filles out the signature? (add to github)</t>
-  </si>
-  <si>
-    <t>Sprint 5
-11/22-12/5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Security stories
+    <t xml:space="preserve">** Previous sprint ***
+Login workflow
+2FA (Can be added anytime)
+**
+Security stories
 - https://github.com/18F/dol-whd-14c/issues/203
 - https://github.com/18F/dol-whd-14c/issues/205
 - https://github.com/18F/dol-whd-14c/issues/174
@@ -319,54 +361,28 @@
 - https://github.com/18F/dol-whd-14c/issues/80
 - https://github.com/18F/dol-whd-14c/issues/84
 - https://github.com/18F/dol-whd-14c/issues/186
+** Madhu to add a few security stories + prioritize
+** RV/LS: Verify which of these are going to be completed before the 12/13 pause.
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Help text
+    <t xml:space="preserve">• Test plan
+Accessibility remediation
+https://github.com/18F/dol-whd-14c/issues/299 (from last sprint)
+https://github.com/18F/dol-whd-14c/issues/297 (blocked)
+Help text
 Helpdesk
 https://github.com/18F/dol-whd-14c/issues/156
 QA Epic testing
 - File upload
 </t>
   </si>
-  <si>
-    <t>PRA submission to OMB</t>
-  </si>
-  <si>
-    <t>DECEMBER</t>
-  </si>
-  <si>
-    <t>Stabilize, Knowledge Transfer, Final Demo/Deploy in DOL</t>
-  </si>
-  <si>
-    <t>QA Testing</t>
-  </si>
-  <si>
-    <t>Sprint 6
-12/6-12/19</t>
-  </si>
-  <si>
-    <t>Demo/Validation of acceptance criteria.</t>
-  </si>
-  <si>
-    <t>Sprint 7
-12/20-1/2</t>
-  </si>
-  <si>
-    <t>critical/ATO Defect fixes done. App deployed in DOL Dev.</t>
-  </si>
-  <si>
-    <t>END OF POP</t>
-  </si>
-  <si>
-    <t>All requirements and acceptance criteria met. App deployed in DOL dev. Knowledge transfer complete. All critical/major defects (ATO, features) are addressed.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,7 +589,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -606,26 +622,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,23 +657,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -850,14 +832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -869,10 +851,10 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -898,7 +880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="2" customFormat="1" ht="63.75">
+    <row r="3" spans="1:10" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -918,7 +900,7 @@
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -938,7 +920,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="114.75">
+    <row r="5" spans="1:10" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -959,7 +941,7 @@
       <c r="H5" s="7"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="127.5">
+    <row r="6" spans="1:10" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="14" t="s">
         <v>8</v>
@@ -977,7 +959,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="409.5" customHeight="1">
+    <row r="7" spans="1:10" s="2" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>1</v>
       </c>
@@ -999,7 +981,7 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="293.25">
+    <row r="8" spans="1:10" s="3" customFormat="1" ht="293.25" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>3</v>
       </c>
@@ -1021,7 +1003,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="127.5">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -1040,10 +1022,12 @@
       <c r="F9" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:10" s="3" customFormat="1" ht="408">
+    <row r="10" spans="1:10" s="3" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>5</v>
       </c>
@@ -1054,18 +1038,18 @@
         <v>34</v>
       </c>
       <c r="D10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:10" s="3" customFormat="1" ht="191.25">
+    <row r="11" spans="1:10" s="3" customFormat="1" ht="293.25" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>6</v>
       </c>
@@ -1073,21 +1057,21 @@
         <v>12</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1">
+    <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>4</v>
       </c>
@@ -1095,19 +1079,19 @@
         <v>8</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
     </row>
-    <row r="13" spans="1:10" ht="25.5">
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1115,17 +1099,17 @@
         <v>12</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="25.5">
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>8</v>
       </c>
@@ -1133,26 +1117,26 @@
         <v>12</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="38.25">
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>4</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E15" s="14"/>
       <c r="F15" s="14"/>
@@ -1167,24 +1151,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1661,17 +1645,50 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36BFE736-C0B4-4AF8-9C17-1890A458A430}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{36BFE736-C0B4-4AF8-9C17-1890A458A430}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bb71f7cc-13ce-42b7-b421-3beaac50452e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="a68e5cfe-8392-4af9-84af-af448c0de71d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50D549BA-0463-4779-B16A-209CF4B97027}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50D549BA-0463-4779-B16A-209CF4B97027}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B34E1A98-487A-4270-B393-2F369D8D6D09}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B34E1A98-487A-4270-B393-2F369D8D6D09}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55883FB9-A121-41BF-9F3C-A28AABBA5F4C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55883FB9-A121-41BF-9F3C-A28AABBA5F4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bb71f7cc-13ce-42b7-b421-3beaac50452e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>